<commit_message>
for eia uploading production
</commit_message>
<xml_diff>
--- a/build/php/UNIVERSEFORMAT.xlsx
+++ b/build/php/UNIVERSEFORMAT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\universe\build\php\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0110BE03-E5DA-465D-AA4B-E7D7F42BDA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543ADC7C-8AF0-4952-85DC-C31A32D848CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E44204E-4644-4721-AE05-8B2604458E58}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
   <si>
     <t>REFERENCE NO.</t>
   </si>
@@ -240,10 +240,13 @@
     <t>2nd Sem</t>
   </si>
   <si>
-    <t>CMR Submission</t>
-  </si>
-  <si>
     <t>CMR Required</t>
+  </si>
+  <si>
+    <t>3rd Sem</t>
+  </si>
+  <si>
+    <t>4th Sem</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -576,6 +579,7 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1011,13 +1015,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28A3988-AF29-40B9-926A-09FFBC92FD40}">
-  <dimension ref="A1:CG5"/>
+  <dimension ref="A1:CI5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="8" ySplit="5" topLeftCell="I6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="5" topLeftCell="BP6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="CG20" sqref="CG20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,10 +1068,11 @@
     <col min="76" max="81" width="16.7109375" customWidth="1"/>
     <col min="82" max="82" width="16.85546875" customWidth="1"/>
     <col min="83" max="85" width="16.7109375" customWidth="1"/>
-    <col min="86" max="87" width="8.85546875" customWidth="1"/>
+    <col min="86" max="86" width="16.140625" customWidth="1"/>
+    <col min="87" max="87" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:87" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>49</v>
       </c>
@@ -1119,7 +1124,7 @@
       <c r="BM1" s="25"/>
       <c r="BN1" s="25"/>
     </row>
-    <row r="2" spans="1:85" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:87" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>50</v>
       </c>
@@ -1200,7 +1205,7 @@
       <c r="BV2" s="48"/>
       <c r="BW2" s="19"/>
     </row>
-    <row r="3" spans="1:85" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:87" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>60</v>
       </c>
@@ -1261,9 +1266,7 @@
       <c r="BT3" s="19"/>
       <c r="BU3" s="19"/>
       <c r="BV3" s="19"/>
-      <c r="BW3" s="45" t="s">
-        <v>68</v>
-      </c>
+      <c r="BW3" s="45"/>
       <c r="BX3" s="45"/>
       <c r="BY3" s="45"/>
       <c r="BZ3" s="45"/>
@@ -1274,8 +1277,10 @@
       <c r="CE3" s="45"/>
       <c r="CF3" s="45"/>
       <c r="CG3" s="46"/>
+      <c r="CH3" s="55"/>
+      <c r="CI3" s="55"/>
     </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
         <v>61</v>
       </c>
@@ -1353,8 +1358,12 @@
         <v>2022</v>
       </c>
       <c r="CG4" s="54"/>
+      <c r="CH4" s="54">
+        <v>2023</v>
+      </c>
+      <c r="CI4" s="54"/>
     </row>
-    <row r="5" spans="1:85" s="15" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:87" s="15" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1578,7 +1587,7 @@
         <v>48</v>
       </c>
       <c r="BW5" s="44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BX5" s="43" t="s">
         <v>66</v>
@@ -1610,9 +1619,16 @@
       <c r="CG5" s="43" t="s">
         <v>67</v>
       </c>
+      <c r="CH5" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="CI5" s="43" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="CH4:CI4"/>
     <mergeCell ref="BW3:CG3"/>
     <mergeCell ref="BJ2:BO2"/>
     <mergeCell ref="BQ2:BS2"/>

</xml_diff>